<commit_message>
Editando excel, criando interface da planilha
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edudu\Desktop\Avulso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77F74736-D5B4-49A1-A902-5048BE1C3D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5144F1B-24B6-4D36-A718-43875D516CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{EEE642CA-D46E-49F9-A632-A0D62952CE38}"/>
   </bookViews>
@@ -24,9 +24,104 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+  <si>
+    <t>Vendas por Setores no 1° Semestre de 2016</t>
+  </si>
+  <si>
+    <t>(Vendas em Milhões)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Histórico de Vendas dos últimos 6 meses </t>
+  </si>
+  <si>
+    <t>Setores</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Baixo</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Atual (Julho)</t>
+  </si>
+  <si>
+    <t>Resultado Mês</t>
+  </si>
+  <si>
+    <t>Desempenho</t>
+  </si>
+  <si>
+    <t>Gráfico Tendência</t>
+  </si>
+  <si>
+    <t>Resultados do Mês</t>
+  </si>
+  <si>
+    <t>Vestuário Feminino</t>
+  </si>
+  <si>
+    <t>Pátio e Jardim</t>
+  </si>
+  <si>
+    <t>Brinquedos</t>
+  </si>
+  <si>
+    <t>Aparelhos Eletrônicos</t>
+  </si>
+  <si>
+    <t>Vestuário para Bebês</t>
+  </si>
+  <si>
+    <t>Vestuário Masculino</t>
+  </si>
+  <si>
+    <t>Vestuário Infantil</t>
+  </si>
+  <si>
+    <t>Móveis</t>
+  </si>
+  <si>
+    <t>Cama e banho</t>
+  </si>
+  <si>
+    <t>Utensilios para Cozinha</t>
+  </si>
+  <si>
+    <t>Casa</t>
+  </si>
+  <si>
+    <t>1° Maior Valor dos "Móveis"</t>
+  </si>
+  <si>
+    <t>2° Maior Valor dos "Móveis"</t>
+  </si>
+  <si>
+    <t>3° Maior Valor dos "Móveis"</t>
+  </si>
+  <si>
+    <t>1° Menor Valor dos "Brinquedos"</t>
+  </si>
+  <si>
+    <t>2° Menor Valor dos "Brinquedo"</t>
+  </si>
+  <si>
+    <t>3° Menor Valor dos "Brinquedo"</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +129,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -51,12 +187,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72,6 +270,137 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Seta: para a Direita 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8DF72E6-7440-47D8-8D38-FE8C662FE1E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="3943350"/>
+          <a:ext cx="1914525" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Valor do Mês Atual (Julho)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Seta: para a Direita 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6BD0B67-4232-4DAC-82BD-5526958B3F4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="4686300"/>
+          <a:ext cx="1933575" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Média</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,12 +700,518 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC106425-ACAA-4732-98B3-0A45ABF688BB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42370</v>
+      </c>
+      <c r="C5" s="3">
+        <v>42401</v>
+      </c>
+      <c r="D5" s="3">
+        <v>42430</v>
+      </c>
+      <c r="E5" s="3">
+        <v>42461</v>
+      </c>
+      <c r="F5" s="3">
+        <v>42491</v>
+      </c>
+      <c r="G5" s="3">
+        <v>42522</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="13">
+        <v>21.2</v>
+      </c>
+      <c r="C8" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="D8" s="14">
+        <v>11</v>
+      </c>
+      <c r="E8" s="14">
+        <v>31.7</v>
+      </c>
+      <c r="F8" s="14">
+        <v>23.8</v>
+      </c>
+      <c r="G8" s="14">
+        <v>12.7</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14">
+        <v>32.6</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="14">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C9" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="D9" s="14">
+        <v>7.6</v>
+      </c>
+      <c r="E9" s="14">
+        <v>2.8</v>
+      </c>
+      <c r="F9" s="14">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G9" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14">
+        <v>16.2</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="14">
+        <v>12.8</v>
+      </c>
+      <c r="C10" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="D10" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="E10" s="14">
+        <v>15.7</v>
+      </c>
+      <c r="F10" s="14">
+        <v>13.7</v>
+      </c>
+      <c r="G10" s="14">
+        <v>15.2</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14">
+        <v>15.7</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="14">
+        <v>13.1</v>
+      </c>
+      <c r="C11" s="14">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D11" s="14">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E11" s="14">
+        <v>19.5</v>
+      </c>
+      <c r="F11" s="14">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G11" s="14">
+        <v>14.7</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14">
+        <v>14.9</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="14">
+        <v>12.5</v>
+      </c>
+      <c r="C12" s="14">
+        <v>5.9</v>
+      </c>
+      <c r="D12" s="14">
+        <v>8.4</v>
+      </c>
+      <c r="E12" s="14">
+        <v>12.9</v>
+      </c>
+      <c r="F12" s="14">
+        <v>9.5</v>
+      </c>
+      <c r="G12" s="14">
+        <v>12.9</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14">
+        <v>14.2</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="14">
+        <v>4.8</v>
+      </c>
+      <c r="C13" s="14">
+        <v>10.5</v>
+      </c>
+      <c r="D13" s="14">
+        <v>7.9</v>
+      </c>
+      <c r="E13" s="14">
+        <v>17.5</v>
+      </c>
+      <c r="F13" s="14">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G13" s="14">
+        <v>11.9</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="14">
+        <v>13.9</v>
+      </c>
+      <c r="C14" s="14">
+        <v>7.5</v>
+      </c>
+      <c r="D14" s="14">
+        <v>11.8</v>
+      </c>
+      <c r="E14" s="14">
+        <v>17.3</v>
+      </c>
+      <c r="F14" s="14">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G14" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14">
+        <v>12.6</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="14">
+        <v>15.8</v>
+      </c>
+      <c r="C15" s="14">
+        <v>11.2</v>
+      </c>
+      <c r="D15" s="14">
+        <v>8.9</v>
+      </c>
+      <c r="E15" s="14">
+        <v>13.7</v>
+      </c>
+      <c r="F15" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G15" s="14">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14">
+        <v>11.4</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="14">
+        <v>15.7</v>
+      </c>
+      <c r="C16" s="14">
+        <v>10.9</v>
+      </c>
+      <c r="D16" s="14">
+        <v>5.8</v>
+      </c>
+      <c r="E16" s="14">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F16" s="14">
+        <v>12.6</v>
+      </c>
+      <c r="G16" s="14">
+        <v>11</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14">
+        <v>11.1</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="14">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C17" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="D17" s="14">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E17" s="14">
+        <v>11.9</v>
+      </c>
+      <c r="F17" s="14">
+        <v>15.9</v>
+      </c>
+      <c r="G17" s="14">
+        <v>8.9</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14">
+        <v>9.9</v>
+      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="14">
+        <v>12.4</v>
+      </c>
+      <c r="C18" s="14">
+        <v>14.9</v>
+      </c>
+      <c r="D18" s="14">
+        <v>11.8</v>
+      </c>
+      <c r="E18" s="14">
+        <v>13</v>
+      </c>
+      <c r="F18" s="14">
+        <v>1.3</v>
+      </c>
+      <c r="G18" s="14">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14">
+        <v>7.5</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="H21" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="H25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="16"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H25:I25"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>